<commit_message>
create new site from Google AI studio code
</commit_message>
<xml_diff>
--- a/1000mProgress.xlsx
+++ b/1000mProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c6047bb88935478/Documents/GitHub/phillongworth.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="13_ncr:1_{4C98DF0E-1A9F-4D1E-8CF7-90BDB97BB963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB35EA55-1413-4D50-80EC-917B2A82BD63}"/>
+  <xr:revisionPtr revIDLastSave="345" documentId="13_ncr:1_{4C98DF0E-1A9F-4D1E-8CF7-90BDB97BB963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67BC6C96-7455-4179-A16F-142FBF341BCF}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A26A407F-7D9C-4DF8-BC8F-7B9BCBDAC91F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Week commencing</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>Number of rides</t>
+  </si>
+  <si>
+    <t>Actual ft</t>
+  </si>
+  <si>
+    <t>Tot mileage</t>
+  </si>
+  <si>
+    <t>Tot feet</t>
   </si>
 </sst>
 </file>
@@ -243,9 +252,6 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -268,6 +274,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -312,17 +321,17 @@
       <calculatedColumnFormula>7+A1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{512D2C8A-F18C-4F98-809D-D85828DFB895}" name="Week no"/>
-    <tableColumn id="11" xr3:uid="{C5DB63B4-CA27-4CD5-9457-234F37536383}" name="Number of rides" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{C5DB63B4-CA27-4CD5-9457-234F37536383}" name="Number of rides" dataDxfId="8">
       <calculatedColumnFormula>COUNTIF(Sheet2!N2:N10,"="&amp;B2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{D4A0D4AB-97ED-4112-B5CB-06508C281FE8}" name="Planned miles"/>
     <tableColumn id="4" xr3:uid="{EAC6E893-F486-42BC-82B8-06BAD98BEEDB}" name="Cumulative miles">
       <calculatedColumnFormula>E1+D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FB8AB5B3-A130-49D3-928F-B7202521E21C}" name="Actual miles (week)" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{FB8AB5B3-A130-49D3-928F-B7202521E21C}" name="Actual miles (week)" dataDxfId="7">
       <calculatedColumnFormula>N2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E880E3D5-CE6B-49FC-A937-540C6B244EEC}" name="Actual miles (cumulative)" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{E880E3D5-CE6B-49FC-A937-540C6B244EEC}" name="Actual miles (cumulative)" dataDxfId="6">
       <calculatedColumnFormula>Sheet2!J2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{874445AB-3682-429E-B15A-EC189D86D12D}" name="Planned ft">
@@ -331,10 +340,10 @@
     <tableColumn id="8" xr3:uid="{4DA5F37D-1FBD-4674-AB4C-7EEA73A9C224}" name="Cumulative ft">
       <calculatedColumnFormula>I1+H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A602CACD-113B-4AA5-9186-99196F898353}" name="Actual ft (week)" dataDxfId="6">
+    <tableColumn id="9" xr3:uid="{A602CACD-113B-4AA5-9186-99196F898353}" name="Actual ft (week)" dataDxfId="5">
       <calculatedColumnFormula>SUMIF(Sheet2!$N$2:$N$100, B2, Sheet2!$I$2:$I$100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7F60711F-AD64-4007-8432-6EDF243B9B9C}" name="Actual ft (cumulative)" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{7F60711F-AD64-4007-8432-6EDF243B9B9C}" name="Actual ft (cumulative)" dataDxfId="4">
       <calculatedColumnFormula>Sheet2!K2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -343,23 +352,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C33CDB7-9962-4FF0-8466-58FFB9D6287A}" name="Table1" displayName="Table1" ref="A1:K100" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C33CDB7-9962-4FF0-8466-58FFB9D6287A}" name="Table1" displayName="Table1" ref="A1:K100" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:K100" xr:uid="{3C33CDB7-9962-4FF0-8466-58FFB9D6287A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I5">
     <sortCondition ref="E1:E5"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F018E7E8-F478-4C2D-B52C-0B5C85D3129F}" name="When" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F018E7E8-F478-4C2D-B52C-0B5C85D3129F}" name="When" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{1101E747-C3D9-4131-8F20-8931C2FCF7CF}" name="Type"/>
     <tableColumn id="3" xr3:uid="{31F23CF9-22F3-4B46-A97C-B264219EB4C3}" name="Sport Type"/>
     <tableColumn id="4" xr3:uid="{5076274C-A0A8-4CEE-A320-5F4FF05DFFB1}" name="Gear"/>
     <tableColumn id="5" xr3:uid="{80211AFC-9813-4AB9-81AF-D505C00C277E}" name="Name"/>
     <tableColumn id="6" xr3:uid="{962F8E50-7DAE-4934-B9E9-C1C8D6F2CCE3}" name="Dist mi"/>
-    <tableColumn id="7" xr3:uid="{70847DCA-CC3D-4031-8C22-F1C0665521DE}" name="Dist (miles)" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{70847DCA-CC3D-4031-8C22-F1C0665521DE}" name="Dist (miles)" dataDxfId="1">
       <calculatedColumnFormula>CONVERT(F2,"m","mi")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{F4E3613D-C261-435A-851F-90AC0685FB0D}" name="Elv ft"/>
-    <tableColumn id="9" xr3:uid="{1BE532E9-3E15-4CD7-8B94-2D3097057AA7}" name="Elv (feet)" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{1BE532E9-3E15-4CD7-8B94-2D3097057AA7}" name="Elv (feet)" dataDxfId="0">
       <calculatedColumnFormula>CONVERT(H2,"m","ft")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{882A6F0D-44E8-4819-8573-19F54CECEA54}" name="Dist (cumulative)"/>
@@ -690,7 +699,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N4" sqref="N4:N7"/>
+      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -737,10 +746,23 @@
       <c r="N1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Q1"/>
-      <c r="R1" s="1"/>
-      <c r="S1"/>
-      <c r="T1"/>
+      <c r="O1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="6">
+        <f>G54</f>
+        <v>85.271111011691715</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="2">
+        <f>K54</f>
+        <v>7502.8976377952749</v>
+      </c>
       <c r="U1"/>
     </row>
     <row r="2" spans="1:21">
@@ -752,7 +774,7 @@
       </c>
       <c r="C2">
         <f>COUNTIF(Sheet2!N2:N10,"="&amp;B2)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -872,7 +894,7 @@
         <v>3000</v>
       </c>
       <c r="J4" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B4, Sheet2!$I$2:$I$100)</f>
+        <f>O4</f>
         <v>2260.4986876640419</v>
       </c>
       <c r="K4" s="2">
@@ -880,8 +902,12 @@
         <v>2260.4986876640419</v>
       </c>
       <c r="N4" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B4, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q2</f>
         <v>27.539544062673983</v>
+      </c>
+      <c r="O4" s="6">
+        <f>Sheet2!R2</f>
+        <v>2260.4986876640419</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -920,7 +946,7 @@
         <v>4000</v>
       </c>
       <c r="J5" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B5, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" ref="J5:J54" si="5">O5</f>
         <v>912.07349081364828</v>
       </c>
       <c r="K5" s="2">
@@ -928,8 +954,12 @@
         <v>3172.5721784776902</v>
       </c>
       <c r="N5" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B5, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q3</f>
         <v>11.517115048118985</v>
+      </c>
+      <c r="O5" s="6">
+        <f>Sheet2!R3</f>
+        <v>912.07349081364828</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -953,11 +983,11 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.11445190089875</v>
       </c>
       <c r="G6" s="5">
         <f>G5+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>39.056659110792964</v>
+        <v>70.171111011691721</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
@@ -968,16 +998,20 @@
         <v>5000</v>
       </c>
       <c r="J6" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B6, Sheet2!$I$2:$I$100)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>2676.3254593175852</v>
       </c>
       <c r="K6" s="2">
         <f>K5+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>3172.5721784776902</v>
+        <v>5848.8976377952749</v>
       </c>
       <c r="N6" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B6, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
+        <f>Sheet2!Q4</f>
+        <v>31.11445190089875</v>
+      </c>
+      <c r="O6" s="6">
+        <f>Sheet2!R4</f>
+        <v>2676.3254593175852</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1001,11 +1035,11 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="1"/>
-        <v>15.194451900898752</v>
+        <v>15.1</v>
       </c>
       <c r="G7" s="5">
         <f>G6+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
@@ -1016,16 +1050,20 @@
         <v>6000</v>
       </c>
       <c r="J7" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B7, Sheet2!$I$2:$I$100)</f>
-        <v>1396.3254593175852</v>
+        <f t="shared" si="5"/>
+        <v>1654</v>
       </c>
       <c r="K7" s="2">
         <f>K6+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N7" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B7, Sheet2!$G$2:$G$100)</f>
-        <v>15.194451900898752</v>
+        <f>Sheet2!Q5</f>
+        <v>15.1</v>
+      </c>
+      <c r="O7" s="6">
+        <f>Sheet2!R5</f>
+        <v>1654</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1053,7 +1091,7 @@
       </c>
       <c r="G8" s="5">
         <f>G7+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
@@ -1064,15 +1102,19 @@
         <v>7000</v>
       </c>
       <c r="J8" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B8, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
         <f>K7+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N8" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B8, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q6</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="6">
+        <f>Sheet2!R6</f>
         <v>0</v>
       </c>
     </row>
@@ -1101,7 +1143,7 @@
       </c>
       <c r="G9" s="5">
         <f>G8+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
@@ -1112,15 +1154,19 @@
         <v>8000</v>
       </c>
       <c r="J9" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B9, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K9" s="2">
         <f>K8+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N9" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B9, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q7</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
+        <f>Sheet2!R7</f>
         <v>0</v>
       </c>
     </row>
@@ -1149,7 +1195,7 @@
       </c>
       <c r="G10" s="5">
         <f>G9+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
@@ -1160,15 +1206,19 @@
         <v>9000</v>
       </c>
       <c r="J10" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B10, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K10" s="2">
         <f>K9+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N10" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B10, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q8</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="6">
+        <f>Sheet2!R8</f>
         <v>0</v>
       </c>
     </row>
@@ -1197,7 +1247,7 @@
       </c>
       <c r="G11" s="5">
         <f>G10+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
@@ -1208,15 +1258,15 @@
         <v>10000</v>
       </c>
       <c r="J11" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B11, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <f>K10+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N11" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B11, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q9</f>
         <v>0</v>
       </c>
     </row>
@@ -1245,7 +1295,7 @@
       </c>
       <c r="G12" s="5">
         <f>G11+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
@@ -1256,15 +1306,15 @@
         <v>11000</v>
       </c>
       <c r="J12" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B12, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K12" s="2">
         <f>K11+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N12" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B12, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q10</f>
         <v>0</v>
       </c>
     </row>
@@ -1293,7 +1343,7 @@
       </c>
       <c r="G13" s="5">
         <f>G12+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
@@ -1304,15 +1354,15 @@
         <v>12000</v>
       </c>
       <c r="J13" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B13, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K13" s="2">
         <f>K12+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N13" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B13, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q11</f>
         <v>0</v>
       </c>
     </row>
@@ -1341,7 +1391,7 @@
       </c>
       <c r="G14" s="5">
         <f>G13+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
@@ -1352,15 +1402,15 @@
         <v>14000</v>
       </c>
       <c r="J14" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B14, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K14" s="2">
         <f>K13+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N14" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B14, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q12</f>
         <v>0</v>
       </c>
     </row>
@@ -1389,7 +1439,7 @@
       </c>
       <c r="G15" s="5">
         <f>G14+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
@@ -1400,15 +1450,15 @@
         <v>16000</v>
       </c>
       <c r="J15" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B15, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K15" s="2">
         <f>K14+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N15" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B15, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q13</f>
         <v>0</v>
       </c>
     </row>
@@ -1437,7 +1487,7 @@
       </c>
       <c r="G16" s="5">
         <f>G15+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
@@ -1448,15 +1498,15 @@
         <v>18000</v>
       </c>
       <c r="J16" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B16, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K16" s="2">
         <f>K15+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N16" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B16, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q14</f>
         <v>0</v>
       </c>
     </row>
@@ -1485,7 +1535,7 @@
       </c>
       <c r="G17" s="5">
         <f>G16+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
@@ -1496,15 +1546,15 @@
         <v>20000</v>
       </c>
       <c r="J17" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B17, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K17" s="2">
         <f>K16+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N17" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B17, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q15</f>
         <v>0</v>
       </c>
     </row>
@@ -1533,7 +1583,7 @@
       </c>
       <c r="G18" s="5">
         <f>G17+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
@@ -1544,15 +1594,15 @@
         <v>22000</v>
       </c>
       <c r="J18" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B18, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K18" s="2">
         <f>K17+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N18" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B18, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q16</f>
         <v>0</v>
       </c>
     </row>
@@ -1581,7 +1631,7 @@
       </c>
       <c r="G19" s="5">
         <f>G18+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -1592,15 +1642,15 @@
         <v>24000</v>
       </c>
       <c r="J19" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B19, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K19" s="2">
         <f>K18+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N19" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B19, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q17</f>
         <v>0</v>
       </c>
     </row>
@@ -1629,7 +1679,7 @@
       </c>
       <c r="G20" s="5">
         <f>G19+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -1640,15 +1690,15 @@
         <v>26000</v>
       </c>
       <c r="J20" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B20, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K20" s="2">
         <f>K19+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N20" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B20, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q18</f>
         <v>0</v>
       </c>
     </row>
@@ -1677,7 +1727,7 @@
       </c>
       <c r="G21" s="5">
         <f>G20+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -1688,15 +1738,15 @@
         <v>28000</v>
       </c>
       <c r="J21" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B21, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K21" s="2">
         <f>K20+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N21" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B21, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q19</f>
         <v>0</v>
       </c>
     </row>
@@ -1725,7 +1775,7 @@
       </c>
       <c r="G22" s="5">
         <f>G21+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -1736,15 +1786,15 @@
         <v>30000</v>
       </c>
       <c r="J22" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B22, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K22" s="2">
         <f>K21+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N22" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B22, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q20</f>
         <v>0</v>
       </c>
     </row>
@@ -1773,7 +1823,7 @@
       </c>
       <c r="G23" s="5">
         <f>G22+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -1784,15 +1834,15 @@
         <v>33000</v>
       </c>
       <c r="J23" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B23, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K23" s="2">
         <f>K22+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N23" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B23, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q21</f>
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1871,7 @@
       </c>
       <c r="G24" s="5">
         <f>G23+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
@@ -1832,15 +1882,15 @@
         <v>36000</v>
       </c>
       <c r="J24" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B24, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K24" s="2">
         <f>K23+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N24" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B24, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q22</f>
         <v>0</v>
       </c>
     </row>
@@ -1869,7 +1919,7 @@
       </c>
       <c r="G25" s="5">
         <f>G24+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
@@ -1880,15 +1930,15 @@
         <v>39000</v>
       </c>
       <c r="J25" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B25, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K25" s="2">
         <f>K24+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N25" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B25, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q23</f>
         <v>0</v>
       </c>
     </row>
@@ -1917,7 +1967,7 @@
       </c>
       <c r="G26" s="5">
         <f>G25+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
@@ -1928,15 +1978,15 @@
         <v>42000</v>
       </c>
       <c r="J26" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B26, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K26" s="2">
         <f>K25+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N26" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B26, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q24</f>
         <v>0</v>
       </c>
     </row>
@@ -1965,7 +2015,7 @@
       </c>
       <c r="G27" s="5">
         <f>G26+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
@@ -1976,15 +2026,15 @@
         <v>45000</v>
       </c>
       <c r="J27" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B27, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K27" s="2">
         <f>K26+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N27" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B27, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q25</f>
         <v>0</v>
       </c>
     </row>
@@ -2013,7 +2063,7 @@
       </c>
       <c r="G28" s="5">
         <f>G27+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
@@ -2024,15 +2074,15 @@
         <v>48000</v>
       </c>
       <c r="J28" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B28, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K28" s="2">
         <f>K27+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N28" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B28, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q26</f>
         <v>0</v>
       </c>
     </row>
@@ -2061,7 +2111,7 @@
       </c>
       <c r="G29" s="5">
         <f>G28+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
@@ -2072,15 +2122,15 @@
         <v>51000</v>
       </c>
       <c r="J29" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B29, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K29" s="2">
         <f>K28+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N29" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B29, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q27</f>
         <v>0</v>
       </c>
     </row>
@@ -2109,7 +2159,7 @@
       </c>
       <c r="G30" s="5">
         <f>G29+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
@@ -2120,15 +2170,15 @@
         <v>54000</v>
       </c>
       <c r="J30" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B30, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K30" s="2">
         <f>K29+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N30" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B30, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q28</f>
         <v>0</v>
       </c>
     </row>
@@ -2157,7 +2207,7 @@
       </c>
       <c r="G31" s="5">
         <f>G30+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
@@ -2168,15 +2218,15 @@
         <v>57000</v>
       </c>
       <c r="J31" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B31, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K31" s="2">
         <f>K30+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N31" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B31, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q29</f>
         <v>0</v>
       </c>
     </row>
@@ -2205,7 +2255,7 @@
       </c>
       <c r="G32" s="5">
         <f>G31+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
@@ -2216,15 +2266,15 @@
         <v>60000</v>
       </c>
       <c r="J32" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B32, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K32" s="2">
         <f>K31+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N32" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B32, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q30</f>
         <v>0</v>
       </c>
     </row>
@@ -2253,7 +2303,7 @@
       </c>
       <c r="G33" s="5">
         <f>G32+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
@@ -2264,15 +2314,15 @@
         <v>63000</v>
       </c>
       <c r="J33" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B33, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K33" s="2">
         <f>K32+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N33" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B33, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q31</f>
         <v>0</v>
       </c>
     </row>
@@ -2301,7 +2351,7 @@
       </c>
       <c r="G34" s="5">
         <f>G33+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
@@ -2312,15 +2362,15 @@
         <v>66000</v>
       </c>
       <c r="J34" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B34, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K34" s="2">
         <f>K33+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N34" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B34, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q32</f>
         <v>0</v>
       </c>
     </row>
@@ -2340,7 +2390,7 @@
         <v>30</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E66" si="5">E34+D35</f>
+        <f t="shared" ref="E35:E54" si="6">E34+D35</f>
         <v>690</v>
       </c>
       <c r="F35" s="5">
@@ -2349,26 +2399,26 @@
       </c>
       <c r="G35" s="5">
         <f>G34+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35:I66" si="6">I34+H35</f>
+        <f t="shared" ref="I35:I54" si="7">I34+H35</f>
         <v>69000</v>
       </c>
       <c r="J35" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B35, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K35" s="2">
         <f>K34+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N35" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B35, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q33</f>
         <v>0</v>
       </c>
     </row>
@@ -2388,7 +2438,7 @@
         <v>30</v>
       </c>
       <c r="E36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>720</v>
       </c>
       <c r="F36" s="5">
@@ -2397,26 +2447,26 @@
       </c>
       <c r="G36" s="5">
         <f>G35+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>72000</v>
       </c>
       <c r="J36" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B36, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K36" s="2">
         <f>K35+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N36" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B36, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q34</f>
         <v>0</v>
       </c>
     </row>
@@ -2436,7 +2486,7 @@
         <v>20</v>
       </c>
       <c r="E37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>740</v>
       </c>
       <c r="F37" s="5">
@@ -2445,26 +2495,26 @@
       </c>
       <c r="G37" s="5">
         <f>G36+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>74000</v>
       </c>
       <c r="J37" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B37, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K37" s="2">
         <f>K36+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N37" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B37, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q35</f>
         <v>0</v>
       </c>
     </row>
@@ -2484,7 +2534,7 @@
         <v>20</v>
       </c>
       <c r="E38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>760</v>
       </c>
       <c r="F38" s="5">
@@ -2493,26 +2543,26 @@
       </c>
       <c r="G38" s="5">
         <f>G37+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76000</v>
       </c>
       <c r="J38" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B38, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K38" s="2">
         <f>K37+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N38" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B38, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q36</f>
         <v>0</v>
       </c>
     </row>
@@ -2532,7 +2582,7 @@
         <v>20</v>
       </c>
       <c r="E39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>780</v>
       </c>
       <c r="F39" s="5">
@@ -2541,26 +2591,26 @@
       </c>
       <c r="G39" s="5">
         <f>G38+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78000</v>
       </c>
       <c r="J39" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B39, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K39" s="2">
         <f>K38+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N39" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B39, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q37</f>
         <v>0</v>
       </c>
     </row>
@@ -2580,7 +2630,7 @@
         <v>20</v>
       </c>
       <c r="E40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>800</v>
       </c>
       <c r="F40" s="5">
@@ -2589,26 +2639,26 @@
       </c>
       <c r="G40" s="5">
         <f>G39+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80000</v>
       </c>
       <c r="J40" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B40, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K40" s="2">
         <f>K39+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N40" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B40, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q38</f>
         <v>0</v>
       </c>
     </row>
@@ -2628,7 +2678,7 @@
         <v>20</v>
       </c>
       <c r="E41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>820</v>
       </c>
       <c r="F41" s="5">
@@ -2637,26 +2687,26 @@
       </c>
       <c r="G41" s="5">
         <f>G40+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>82000</v>
       </c>
       <c r="J41" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B41, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K41" s="2">
         <f>K40+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N41" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B41, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q39</f>
         <v>0</v>
       </c>
     </row>
@@ -2676,7 +2726,7 @@
         <v>20</v>
       </c>
       <c r="E42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>840</v>
       </c>
       <c r="F42" s="5">
@@ -2685,26 +2735,26 @@
       </c>
       <c r="G42" s="5">
         <f>G41+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>84000</v>
       </c>
       <c r="J42" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B42, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K42" s="2">
         <f>K41+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N42" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B42, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q40</f>
         <v>0</v>
       </c>
     </row>
@@ -2724,7 +2774,7 @@
         <v>20</v>
       </c>
       <c r="E43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>860</v>
       </c>
       <c r="F43" s="5">
@@ -2733,26 +2783,26 @@
       </c>
       <c r="G43" s="5">
         <f>G42+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>86000</v>
       </c>
       <c r="J43" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B43, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K43" s="2">
         <f>K42+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N43" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B43, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q41</f>
         <v>0</v>
       </c>
     </row>
@@ -2772,7 +2822,7 @@
         <v>20</v>
       </c>
       <c r="E44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>880</v>
       </c>
       <c r="F44" s="5">
@@ -2781,26 +2831,26 @@
       </c>
       <c r="G44" s="5">
         <f>G43+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>88000</v>
       </c>
       <c r="J44" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B44, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K44" s="2">
         <f>K43+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N44" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B44, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q42</f>
         <v>0</v>
       </c>
     </row>
@@ -2820,7 +2870,7 @@
         <v>20</v>
       </c>
       <c r="E45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>900</v>
       </c>
       <c r="F45" s="5">
@@ -2829,26 +2879,26 @@
       </c>
       <c r="G45" s="5">
         <f>G44+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>90000</v>
       </c>
       <c r="J45" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B45, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K45" s="2">
         <f>K44+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N45" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B45, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q43</f>
         <v>0</v>
       </c>
     </row>
@@ -2868,7 +2918,7 @@
         <v>20</v>
       </c>
       <c r="E46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>920</v>
       </c>
       <c r="F46" s="5">
@@ -2877,26 +2927,26 @@
       </c>
       <c r="G46" s="5">
         <f>G45+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>92000</v>
       </c>
       <c r="J46" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B46, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K46" s="2">
         <f>K45+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N46" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B46, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q44</f>
         <v>0</v>
       </c>
     </row>
@@ -2916,7 +2966,7 @@
         <v>20</v>
       </c>
       <c r="E47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>940</v>
       </c>
       <c r="F47" s="5">
@@ -2925,26 +2975,26 @@
       </c>
       <c r="G47" s="5">
         <f>G46+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>94000</v>
       </c>
       <c r="J47" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B47, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K47" s="2">
         <f>K46+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N47" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B47, Sheet2!$G$2:$G$100)</f>
+        <f>Sheet2!Q45</f>
         <v>0</v>
       </c>
     </row>
@@ -2964,7 +3014,7 @@
         <v>20</v>
       </c>
       <c r="E48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>960</v>
       </c>
       <c r="F48" s="5">
@@ -2973,30 +3023,30 @@
       </c>
       <c r="G48" s="5">
         <f>G47+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>96000</v>
       </c>
       <c r="J48" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B48, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K48" s="2">
         <f>K47+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N48" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B48, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14">
+        <f>Sheet2!Q46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" s="1">
         <f t="shared" si="4"/>
         <v>45991</v>
@@ -3012,7 +3062,7 @@
         <v>20</v>
       </c>
       <c r="E49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>980</v>
       </c>
       <c r="F49" s="5">
@@ -3021,30 +3071,30 @@
       </c>
       <c r="G49" s="5">
         <f>G48+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
       <c r="I49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>98000</v>
       </c>
       <c r="J49" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B49, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K49" s="2">
         <f>K48+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N49" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B49, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <f>Sheet2!Q47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="1">
         <f t="shared" si="4"/>
         <v>45998</v>
@@ -3060,7 +3110,7 @@
         <v>10</v>
       </c>
       <c r="E50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>990</v>
       </c>
       <c r="F50" s="5">
@@ -3069,30 +3119,30 @@
       </c>
       <c r="G50" s="5">
         <f>G49+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="I50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>99000</v>
       </c>
       <c r="J50" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B50, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K50" s="2">
         <f>K49+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N50" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B50, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <f>Sheet2!Q48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" s="1">
         <f t="shared" si="4"/>
         <v>46005</v>
@@ -3108,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="E51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1000</v>
       </c>
       <c r="F51" s="5">
@@ -3117,30 +3167,30 @@
       </c>
       <c r="G51" s="5">
         <f>G50+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="I51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100000</v>
       </c>
       <c r="J51" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B51, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K51" s="2">
         <f>K50+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N51" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B51, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <f>Sheet2!Q49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" s="1">
         <f t="shared" si="4"/>
         <v>46012</v>
@@ -3156,7 +3206,7 @@
         <v>10</v>
       </c>
       <c r="E52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1010</v>
       </c>
       <c r="F52" s="5">
@@ -3165,30 +3215,30 @@
       </c>
       <c r="G52" s="5">
         <f>G51+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="I52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>101000</v>
       </c>
       <c r="J52" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B52, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K52" s="2">
         <f>K51+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N52" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B52, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <f>Sheet2!Q50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" s="1">
         <f t="shared" si="4"/>
         <v>46019</v>
@@ -3204,7 +3254,7 @@
         <v>10</v>
       </c>
       <c r="E53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1020</v>
       </c>
       <c r="F53" s="5">
@@ -3213,30 +3263,30 @@
       </c>
       <c r="G53" s="5">
         <f>G52+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="I53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>102000</v>
       </c>
       <c r="J53" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B53, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K53" s="2">
         <f>K52+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N53" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B53, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <f>Sheet2!Q51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
       <c r="A54" s="1">
         <f>7+A53</f>
         <v>46026</v>
@@ -3252,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="E54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1030</v>
       </c>
       <c r="F54" s="5">
@@ -3261,30 +3311,30 @@
       </c>
       <c r="G54" s="5">
         <f>G53+Table2[[#This Row],[Actual miles (week)]]</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H54">
         <f t="shared" si="2"/>
         <v>1000</v>
       </c>
       <c r="I54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>103000</v>
       </c>
       <c r="J54" s="2">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B54, Sheet2!$I$2:$I$100)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K54" s="2">
         <f>K53+Table2[[#This Row],[Actual ft (week)]]</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="N54" s="5">
-        <f>SUMIF(Sheet2!$N$2:$N$100, B54, Sheet2!$G$2:$G$100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <f>Sheet2!Q52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="D55">
         <f>SUM(D2:D54)</f>
         <v>1030</v>
@@ -3292,6 +3342,22 @@
       <c r="H55">
         <f>SUM(H2:H54)</f>
         <v>103000</v>
+      </c>
+      <c r="L55">
+        <f t="shared" ref="L55:O55" si="8">SUM(L2:L54)</f>
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="8"/>
+        <v>85.271111011691715</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="8"/>
+        <v>7502.8976377952749</v>
       </c>
     </row>
   </sheetData>
@@ -3304,11 +3370,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32516192-437D-4BCA-AAA6-A1C9DF4AFE1A}">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1:T1048576"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3321,7 +3387,7 @@
     <col min="10" max="11" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" ht="29.4" thickBot="1">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="29.4" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -3368,7 +3434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:18" ht="15" thickBot="1">
       <c r="A2" s="4">
         <v>45672.394525462965</v>
       </c>
@@ -3415,15 +3481,19 @@
         <v>3</v>
       </c>
       <c r="P2" cm="1">
-        <f t="array" ref="P2:P6">_xlfn.UNIQUE(N2:N100)</f>
+        <f t="array" ref="P2:P7">_xlfn.UNIQUE(N2:N100)</f>
         <v>3</v>
       </c>
       <c r="Q2" s="9">
         <f>SUMIF($N$2:$N$10, P2, $G$2:$G$10)</f>
         <v>27.539544062673983</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1">
+      <c r="R2" s="9">
+        <f>SUMIF($N$2:$N$10, P2, $I$2:$I$10)</f>
+        <v>2260.4986876640419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1">
       <c r="A3" s="4">
         <v>45674.343009259261</v>
       </c>
@@ -3473,11 +3543,15 @@
         <v>4</v>
       </c>
       <c r="Q3" s="9">
-        <f t="shared" ref="Q3:Q4" si="1">SUMIF($N$2:$N$10, P3, $G$2:$G$10)</f>
+        <f t="shared" ref="Q3:Q6" si="1">SUMIF($N$2:$N$10, P3, $G$2:$G$10)</f>
         <v>11.517115048118985</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1">
+      <c r="R3" s="9">
+        <f t="shared" ref="R3:R8" si="2">SUMIF($N$2:$N$10, P3, $I$2:$I$10)</f>
+        <v>912.07349081364828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15" thickBot="1">
       <c r="A4" s="4">
         <v>45678.342546296299</v>
       </c>
@@ -3528,10 +3602,14 @@
       </c>
       <c r="Q4" s="9">
         <f t="shared" si="1"/>
-        <v>15.194451900898752</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1">
+        <v>31.11445190089875</v>
+      </c>
+      <c r="R4" s="9">
+        <f t="shared" si="2"/>
+        <v>2676.3254593175852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15" thickBot="1">
       <c r="A5" s="4">
         <v>45691.380266203705</v>
       </c>
@@ -3578,55 +3656,100 @@
         <v>6</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="9">
-        <f>SUMIF($N$2:$N$10, P5, $G$2:$G$10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1">
-      <c r="A6" s="4"/>
-      <c r="G6" s="6"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="2"/>
+        <f t="shared" si="1"/>
+        <v>15.1</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="2"/>
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickBot="1">
+      <c r="A6" s="4">
+        <v>45695</v>
+      </c>
+      <c r="E6">
+        <v>1005</v>
+      </c>
+      <c r="G6" s="6">
+        <v>15.92</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1280</v>
+      </c>
+      <c r="J6" s="6">
+        <f>J5+Table1[[#This Row],[Dist (miles)]]</f>
+        <v>70.171111011691721</v>
+      </c>
+      <c r="K6" s="2">
+        <f>K5+Table1[[#This Row],[Elv (feet)]]</f>
+        <v>5848.8976377952749</v>
+      </c>
       <c r="N6">
         <f>WEEKNUM(Table1[[#This Row],[When]],2)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P6">
         <v>1</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6" s="9">
-        <f t="shared" ref="Q6:Q8" si="2">SUMIF($N$2:$N$10, P6, $G$2:$G$10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1">
-      <c r="A7" s="4"/>
-      <c r="G7" s="6"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="2"/>
+        <f t="shared" ref="Q6" si="3">SUMIF($N$2:$N$10, P6, $G$2:$G$10)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" ref="R6" si="4">SUMIF($N$2:$N$10, P6, $I$2:$I$10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15" thickBot="1">
+      <c r="A7" s="4">
+        <v>45700</v>
+      </c>
+      <c r="E7">
+        <v>1006</v>
+      </c>
+      <c r="G7" s="6">
+        <v>15.1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1654</v>
+      </c>
+      <c r="J7" s="6">
+        <f>J6+Table1[[#This Row],[Dist (miles)]]</f>
+        <v>85.271111011691715</v>
+      </c>
+      <c r="K7" s="2">
+        <f>K6+Table1[[#This Row],[Elv (feet)]]</f>
+        <v>7502.8976377952749</v>
+      </c>
       <c r="N7">
         <f>WEEKNUM(Table1[[#This Row],[When]],2)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
       </c>
       <c r="Q7" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1">
+        <f t="shared" ref="Q7:Q8" si="5">SUMIF($N$2:$N$10, P7, $G$2:$G$10)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1">
       <c r="A8" s="4"/>
       <c r="G8" s="6"/>
       <c r="I8" s="2"/>
@@ -3641,60 +3764,64 @@
         <v>1</v>
       </c>
       <c r="Q8" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="4"/>
       <c r="G9" s="6"/>
       <c r="I9" s="2"/>
       <c r="J9" s="6"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" s="4"/>
       <c r="G10" s="6"/>
       <c r="I10" s="2"/>
       <c r="J10" s="6"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" s="4"/>
       <c r="G11" s="6"/>
       <c r="I11" s="2"/>
       <c r="J11" s="6"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12" s="4"/>
       <c r="G12" s="6"/>
       <c r="I12" s="2"/>
       <c r="J12" s="6"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" s="4"/>
       <c r="G13" s="6"/>
       <c r="I13" s="2"/>
       <c r="J13" s="6"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" s="4"/>
       <c r="G14" s="6"/>
       <c r="I14" s="2"/>
       <c r="J14" s="6"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="4"/>
       <c r="G15" s="6"/>
       <c r="I15" s="2"/>
       <c r="J15" s="6"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" s="4"/>
       <c r="G16" s="6"/>
       <c r="I16" s="2"/>
@@ -4297,12 +4424,12 @@
       <c r="F101" s="5"/>
       <c r="G101" s="5">
         <f>SUBTOTAL(109,Table1[Dist (miles)])</f>
-        <v>54.251111011691719</v>
+        <v>85.271111011691715</v>
       </c>
       <c r="H101" s="5"/>
       <c r="I101" s="5">
         <f>SUBTOTAL(109,Table1[Elv (feet)])</f>
-        <v>4568.8976377952749</v>
+        <v>7502.8976377952749</v>
       </c>
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>

</xml_diff>